<commit_message>
Next stage of edits
</commit_message>
<xml_diff>
--- a/data/nlc_factoid_training.xlsx
+++ b/data/nlc_factoid_training.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="4" r:id="rId1"/>
@@ -12,8 +12,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">original!$A$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Training!$D$1:$D$34</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="0">Training!$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Training!#REF!</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">Training!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="101">
   <si>
     <t>Input</t>
   </si>
@@ -48,18 +48,6 @@
     <t>Do you know the population of *?</t>
   </si>
   <si>
-    <t>What's the height of *?</t>
-  </si>
-  <si>
-    <t>Do you know the height of *?</t>
-  </si>
-  <si>
-    <t>How tall is *?</t>
-  </si>
-  <si>
-    <t>Do you know how tall * is?</t>
-  </si>
-  <si>
     <t>place</t>
   </si>
   <si>
@@ -78,9 +66,6 @@
     <t>population</t>
   </si>
   <si>
-    <t>height</t>
-  </si>
-  <si>
     <t>person</t>
   </si>
   <si>
@@ -123,9 +108,6 @@
     <t>Tell me who is *'s husband.</t>
   </si>
   <si>
-    <t>Tell me the height of *.</t>
-  </si>
-  <si>
     <t>Tell me the population of *.</t>
   </si>
   <si>
@@ -150,9 +132,6 @@
     <t>place-population</t>
   </si>
   <si>
-    <t>place-height</t>
-  </si>
-  <si>
     <t>person-spouse</t>
   </si>
   <si>
@@ -177,16 +156,178 @@
     <t>Cause of *?</t>
   </si>
   <si>
-    <t>place-person</t>
-  </si>
-  <si>
-    <t>What is *'s height?</t>
-  </si>
-  <si>
-    <t>place-person-height</t>
-  </si>
-  <si>
-    <t>health_condition-cause</t>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>Where was * born?</t>
+  </si>
+  <si>
+    <t>Can you tell me the ago of *?</t>
+  </si>
+  <si>
+    <t>Can you tell me how old * is?</t>
+  </si>
+  <si>
+    <t>What's the birthdate for *?</t>
+  </si>
+  <si>
+    <t>What is *'s birthdate?</t>
+  </si>
+  <si>
+    <t>When was * born?</t>
+  </si>
+  <si>
+    <t>What age is *?</t>
+  </si>
+  <si>
+    <t>How old is *?</t>
+  </si>
+  <si>
+    <t>What's the birthplace of *?</t>
+  </si>
+  <si>
+    <t>Tell me where * was born.</t>
+  </si>
+  <si>
+    <t>What is the birthplace of *?</t>
+  </si>
+  <si>
+    <t>In which country was * born?</t>
+  </si>
+  <si>
+    <t>In which state was * born?</t>
+  </si>
+  <si>
+    <t>In which city was * born?</t>
+  </si>
+  <si>
+    <t>birthplace</t>
+  </si>
+  <si>
+    <t>schooling</t>
+  </si>
+  <si>
+    <t>Where did * go to school?</t>
+  </si>
+  <si>
+    <t>Which schools did * attend?</t>
+  </si>
+  <si>
+    <t>Which schools did * go to?</t>
+  </si>
+  <si>
+    <t>Which university did * attend?</t>
+  </si>
+  <si>
+    <t>Which university did * go to?</t>
+  </si>
+  <si>
+    <t>Which college did * attend?</t>
+  </si>
+  <si>
+    <t>Which college did * go to?</t>
+  </si>
+  <si>
+    <t>Where did * attend college?</t>
+  </si>
+  <si>
+    <t>Where did * attend university?</t>
+  </si>
+  <si>
+    <t>What is *'s alma mater?</t>
+  </si>
+  <si>
+    <t>How many people live in *?</t>
+  </si>
+  <si>
+    <t>areacode</t>
+  </si>
+  <si>
+    <t>What's the area code for *</t>
+  </si>
+  <si>
+    <t>what is the areacode for *?</t>
+  </si>
+  <si>
+    <t>What's the telephone area code for *</t>
+  </si>
+  <si>
+    <t>What's the dialing code for *</t>
+  </si>
+  <si>
+    <t>Who is the mayor of *?</t>
+  </si>
+  <si>
+    <t>Who is the leader of *?</t>
+  </si>
+  <si>
+    <t>Who is the governor of *?</t>
+  </si>
+  <si>
+    <t>governor_mayor</t>
+  </si>
+  <si>
+    <t>completion_date</t>
+  </si>
+  <si>
+    <t>When was * built?</t>
+  </si>
+  <si>
+    <t>When was the construciton of * completed by?</t>
+  </si>
+  <si>
+    <t>What year was * buit?</t>
+  </si>
+  <si>
+    <t>What was the construction date of *?</t>
+  </si>
+  <si>
+    <t>How much is * worth?</t>
+  </si>
+  <si>
+    <t>How much money does * have?</t>
+  </si>
+  <si>
+    <t>What is *'s net worth?</t>
+  </si>
+  <si>
+    <t>net_worth</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>condition_cause</t>
+  </si>
+  <si>
+    <t>Is there a cure for *?</t>
+  </si>
+  <si>
+    <t>How do I treat *?</t>
+  </si>
+  <si>
+    <t>place-completion_date</t>
+  </si>
+  <si>
+    <t>person-birthdate</t>
+  </si>
+  <si>
+    <t>person-birthplace</t>
+  </si>
+  <si>
+    <t>person-schooling</t>
+  </si>
+  <si>
+    <t>place-areacode</t>
+  </si>
+  <si>
+    <t>place-governor_mayor</t>
+  </si>
+  <si>
+    <t>person-net_worth</t>
+  </si>
+  <si>
+    <t>health-condition_cause</t>
   </si>
 </sst>
 </file>
@@ -232,7 +373,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -240,8 +381,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="219">
+  <cellStyleXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -461,15 +611,75 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="219">
+  <cellStyles count="277">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -579,6 +789,43 @@
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -688,6 +935,27 @@
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1017,436 +1285,592 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>51</v>
       </c>
-      <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>26</v>
-      </c>
       <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>46</v>
       </c>
       <c r="B34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
         <v>53</v>
       </c>
-      <c r="D34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" t="s">
-        <v>53</v>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>87</v>
+      </c>
+      <c r="B63" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B64" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1462,10 +1886,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD37"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1482,13 +1906,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1500,10 +1924,10 @@
         <v>place-capital</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1511,29 +1935,29 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B24" si="0">CONCATENATE(C3,"-",D3,IF(E3="","",CONCATENATE("-",E3)))</f>
+        <f t="shared" ref="B3:B22" si="0">CONCATENATE(C3,"-",D3,IF(E3="","",CONCATENATE("-",E3)))</f>
         <v>place-capital</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" ref="B4" si="1">CONCATENATE(C4,"-",D4,IF(E4="","",CONCATENATE("-",E4)))</f>
         <v>place-capital</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1545,25 +1969,25 @@
         <v>place-capital</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>place-capital</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1575,10 +1999,10 @@
         <v>place-population</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1590,10 +2014,10 @@
         <v>place-population</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1605,472 +2029,970 @@
         <v>place-population</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="B10" s="2" t="str">
+        <f t="shared" ref="B10" si="2">CONCATENATE(C10,"-",D10,IF(E10="","",CONCATENATE("-",E10)))</f>
+        <v>place-population</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>place-population</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>place-person-height</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>place-person-height</v>
+        <v>place-completion_date</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="B13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>place-person-height</v>
+        <v>place-completion_date</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>place-person-height</v>
+        <v>place-completion_date</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>place-person-height</v>
+        <v>place-completion_date</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f t="shared" ref="B16" si="2">CONCATENATE(C16,"-",D16,IF(E16="","",CONCATENATE("-",E16)))</f>
-        <v>place-person-height</v>
+        <f t="shared" si="0"/>
+        <v>person-spouse</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>place-person-height</v>
+        <v>person-spouse</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>person-spouse</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>person-spouse</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>person-spouse</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>person-spouse</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>person-spouse</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B23:B25" si="3">CONCATENATE(C23,"-",D23,IF(E23="","",CONCATENATE("-",E23)))</f>
         <v>person-spouse</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>person-spouse</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2" t="str">
-        <f t="shared" ref="B25:B27" si="3">CONCATENATE(C25,"-",D25,IF(E25="","",CONCATENATE("-",E25)))</f>
+        <f t="shared" si="3"/>
         <v>person-spouse</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B26" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>person-spouse</v>
+        <f>CONCATENATE(C26,"-",D26,IF(E23="","",CONCATENATE("-",E23)))</f>
+        <v>person-children</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B27" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>person-spouse</v>
+        <f>CONCATENATE(C27,"-",D27,IF(E24="","",CONCATENATE("-",E24)))</f>
+        <v>person-children</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B28" s="2" t="str">
         <f>CONCATENATE(C28,"-",D28,IF(E25="","",CONCATENATE("-",E25)))</f>
         <v>person-children</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B29" s="2" t="str">
         <f>CONCATENATE(C29,"-",D29,IF(E26="","",CONCATENATE("-",E26)))</f>
         <v>person-children</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B30" s="2" t="str">
-        <f>CONCATENATE(C30,"-",D30,IF(E27="","",CONCATENATE("-",E27)))</f>
-        <v>person-children</v>
+        <f t="shared" ref="B30:B45" si="4">CONCATENATE(C30,"-",D30,IF(E30="","",CONCATENATE("-",E30)))</f>
+        <v>person-birthdate</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B31" s="2" t="str">
-        <f>CONCATENATE(C31,"-",D31,IF(E28="","",CONCATENATE("-",E28)))</f>
-        <v>person-children</v>
+        <f t="shared" ref="B31:B34" si="5">CONCATENATE(C31,"-",D31,IF(E31="","",CONCATENATE("-",E31)))</f>
+        <v>person-birthdate</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="B32" s="2" t="str">
-        <f t="shared" ref="B32:B53" si="4">CONCATENATE(C32,"-",D32,IF(E32="","",CONCATENATE("-",E32)))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
+        <f t="shared" si="5"/>
+        <v>person-birthdate</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="B33" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
+        <f t="shared" si="5"/>
+        <v>person-birthdate</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="B34" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
+        <f t="shared" si="5"/>
+        <v>person-birthdate</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="B35" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
+        <f t="shared" ref="B35:B36" si="6">CONCATENATE(C35,"-",D35,IF(E35="","",CONCATENATE("-",E35)))</f>
+        <v>person-birthdate</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="B36" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
+        <f t="shared" si="6"/>
+        <v>person-birthdate</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="B37" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
+        <v>person-birthplace</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="B38" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
+        <v>person-birthplace</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="B39" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
+        <v>person-birthplace</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="B40" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2">
+        <v>person-birthplace</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="B41" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2">
+        <v>person-birthplace</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="B42" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2">
+        <v>person-birthplace</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="B43" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2">
+        <v>person-birthplace</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="B44" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2">
+        <v>person-birthplace</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B45" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2">
+        <v>person-schooling</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="B46" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2">
+        <f t="shared" ref="B46:B53" si="7">CONCATENATE(C46,"-",D46,IF(E46="","",CONCATENATE("-",E46)))</f>
+        <v>person-schooling</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="B47" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2">
+        <f t="shared" si="7"/>
+        <v>person-schooling</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="B48" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
+        <f t="shared" si="7"/>
+        <v>person-schooling</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="B49" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
+        <f t="shared" si="7"/>
+        <v>person-schooling</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="B50" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
+        <f t="shared" si="7"/>
+        <v>person-schooling</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B51" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2">
+        <f t="shared" si="7"/>
+        <v>person-schooling</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="B52" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2">
+        <f t="shared" si="7"/>
+        <v>person-schooling</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="B53" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
+        <f t="shared" si="7"/>
+        <v>person-schooling</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" s="2" t="str">
+        <f t="shared" ref="B54:B55" si="8">CONCATENATE(C54,"-",D54,IF(E54="","",CONCATENATE("-",E54)))</f>
+        <v>person-schooling</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>place-areacode</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" s="2" t="str">
+        <f t="shared" ref="B56:B58" si="9">CONCATENATE(C56,"-",D56,IF(E56="","",CONCATENATE("-",E56)))</f>
+        <v>place-areacode</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>place-areacode</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>place-areacode</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="2" t="str">
+        <f t="shared" ref="B59:B62" si="10">CONCATENATE(C59,"-",D59,IF(E59="","",CONCATENATE("-",E59)))</f>
+        <v>place-governor_mayor</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>place-governor_mayor</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>place-governor_mayor</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>person-net_worth</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="2" t="str">
+        <f t="shared" ref="B63:B70" si="11">CONCATENATE(C63,"-",D63,IF(E63="","",CONCATENATE("-",E63)))</f>
+        <v>person-net_worth</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>person-net_worth</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>37</v>
+      </c>
+      <c r="B65" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>40</v>
+      </c>
+      <c r="B68" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" s="2" t="str">
+        <f t="shared" ref="B71" si="12">CONCATENATE(C71,"-",D71,IF(E71="","",CONCATENATE("-",E71)))</f>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="2" t="str">
+        <f t="shared" ref="B72" si="13">CONCATENATE(C72,"-",D72,IF(E72="","",CONCATENATE("-",E72)))</f>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" s="2" t="str">
+        <f t="shared" ref="B73" si="14">CONCATENATE(C73,"-",D73,IF(E73="","",CONCATENATE("-",E73)))</f>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switching to more compact dbpedia calls from pipelines
</commit_message>
<xml_diff>
--- a/data/nlc_factoid_training.xlsx
+++ b/data/nlc_factoid_training.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="31620" windowHeight="20040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="105">
   <si>
     <t>Input</t>
   </si>
@@ -328,6 +328,18 @@
   </si>
   <si>
     <t>health-condition_cause</t>
+  </si>
+  <si>
+    <t>Why do people catch the *?</t>
+  </si>
+  <si>
+    <t>What are common causes for *?</t>
+  </si>
+  <si>
+    <t>What are common reasons for people to get *?</t>
+  </si>
+  <si>
+    <t>How does a person get *?</t>
   </si>
 </sst>
 </file>
@@ -391,7 +403,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="277">
+  <cellStyleXfs count="285">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -668,6 +680,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
@@ -679,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="277">
+  <cellStyles count="285">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -826,6 +846,10 @@
     <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -956,6 +980,10 @@
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1287,7 +1315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
@@ -1886,10 +1914,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77:D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2992,6 +3020,66 @@
         <v>89</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74" s="2" t="str">
+        <f t="shared" ref="B74" si="15">CONCATENATE(C74,"-",D74,IF(E74="","",CONCATENATE("-",E74)))</f>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B75" s="2" t="str">
+        <f t="shared" ref="B75:B76" si="16">CONCATENATE(C75,"-",D75,IF(E75="","",CONCATENATE("-",E75)))</f>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" s="2" t="str">
+        <f t="shared" ref="B77" si="17">CONCATENATE(C77,"-",D77,IF(E77="","",CONCATENATE("-",E77)))</f>
+        <v>health-condition_cause</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Height and elevation now supported
</commit_message>
<xml_diff>
--- a/data/nlc_factoid_training.xlsx
+++ b/data/nlc_factoid_training.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="112">
   <si>
     <t>Input</t>
   </si>
@@ -343,6 +343,24 @@
   </si>
   <si>
     <t>On what date was * born?</t>
+  </si>
+  <si>
+    <t>How tall is *?</t>
+  </si>
+  <si>
+    <t>What's the height of *?</t>
+  </si>
+  <si>
+    <t>How high is *?</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>place-height</t>
+  </si>
+  <si>
+    <t>What's the elevation of *?</t>
   </si>
 </sst>
 </file>
@@ -406,7 +424,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="287">
+  <cellStyleXfs count="297">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -683,6 +701,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -704,7 +732,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="287">
+  <cellStyles count="297">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -856,6 +884,11 @@
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -991,6 +1024,11 @@
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1320,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1566,7 +1604,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
         <v>94</v>
@@ -1574,7 +1612,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
         <v>94</v>
@@ -1582,7 +1620,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
         <v>94</v>
@@ -1590,7 +1628,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
         <v>94</v>
@@ -1598,7 +1636,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
         <v>94</v>
@@ -1606,7 +1644,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
         <v>94</v>
@@ -1614,15 +1652,15 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
         <v>95</v>
@@ -1630,7 +1668,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
         <v>95</v>
@@ -1638,7 +1676,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
         <v>95</v>
@@ -1646,7 +1684,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
         <v>95</v>
@@ -1654,7 +1692,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
         <v>95</v>
@@ -1662,7 +1700,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
         <v>95</v>
@@ -1670,7 +1708,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
         <v>95</v>
@@ -1678,15 +1716,15 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
         <v>96</v>
@@ -1694,7 +1732,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
         <v>96</v>
@@ -1702,7 +1740,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
         <v>96</v>
@@ -1710,7 +1748,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
         <v>96</v>
@@ -1718,7 +1756,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
         <v>96</v>
@@ -1726,7 +1764,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
         <v>96</v>
@@ -1734,7 +1772,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
         <v>96</v>
@@ -1742,7 +1780,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
         <v>96</v>
@@ -1750,7 +1788,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
         <v>96</v>
@@ -1758,15 +1796,15 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B55" t="s">
         <v>97</v>
@@ -1774,7 +1812,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B56" t="s">
         <v>97</v>
@@ -1782,7 +1820,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B57" t="s">
         <v>97</v>
@@ -1790,15 +1828,15 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
         <v>98</v>
@@ -1806,7 +1844,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B60" t="s">
         <v>98</v>
@@ -1814,15 +1852,15 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
         <v>99</v>
@@ -1830,7 +1868,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
         <v>99</v>
@@ -1838,15 +1876,15 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B64" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B65" t="s">
         <v>100</v>
@@ -1854,7 +1892,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B66" t="s">
         <v>100</v>
@@ -1862,7 +1900,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B67" t="s">
         <v>100</v>
@@ -1870,7 +1908,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B68" t="s">
         <v>100</v>
@@ -1878,7 +1916,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B69" t="s">
         <v>100</v>
@@ -1886,7 +1924,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="B70" t="s">
         <v>100</v>
@@ -1894,7 +1932,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B71" t="s">
         <v>100</v>
@@ -1906,6 +1944,70 @@
       </c>
       <c r="B72" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>102</v>
+      </c>
+      <c r="B75" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>107</v>
+      </c>
+      <c r="B79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1921,10 +2023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:D31"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3103,6 +3205,66 @@
       </c>
       <c r="D78" s="2" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79" s="2" t="str">
+        <f t="shared" ref="B79:B81" si="19">CONCATENATE(C79,"-",D79,IF(E79="","",CONCATENATE("-",E79)))</f>
+        <v>place-height</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B80" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>place-height</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>place-height</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" s="2" t="str">
+        <f t="shared" ref="B82" si="20">CONCATENATE(C82,"-",D82,IF(E82="","",CONCATENATE("-",E82)))</f>
+        <v>place-height</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>